<commit_message>
Update cctest/scripts/tests/SPS_MPS/doc/main_loads.xlsx to define circuit simulator characteristics
</commit_message>
<xml_diff>
--- a/cctest/scripts/tests/SPS_MPS/doc/main_loads.xlsx
+++ b/cctest/scripts/tests/SPS_MPS/doc/main_loads.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>OHMS_SER</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>10% overrange</t>
+  </si>
+  <si>
+    <t>Sim R</t>
+  </si>
+  <si>
+    <t>Sim C</t>
+  </si>
+  <si>
+    <t>SIM DCCT.x.GAIN</t>
   </si>
 </sst>
 </file>
@@ -90,15 +99,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,14 +121,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -219,11 +255,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42710528"/>
-        <c:axId val="42708992"/>
+        <c:axId val="76279808"/>
+        <c:axId val="76281344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42710528"/>
+        <c:axId val="76279808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -233,12 +269,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42708992"/>
+        <c:crossAx val="76281344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42708992"/>
+        <c:axId val="76281344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -249,7 +285,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42710528"/>
+        <c:crossAx val="76279808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -356,11 +392,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80070528"/>
-        <c:axId val="80068992"/>
+        <c:axId val="77882496"/>
+        <c:axId val="77884032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80070528"/>
+        <c:axId val="77882496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -370,12 +406,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80068992"/>
+        <c:crossAx val="77884032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80068992"/>
+        <c:axId val="77884032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80070528"/>
+        <c:crossAx val="77882496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -413,8 +449,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -832,138 +868,175 @@
   <dimension ref="B3:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B3" sqref="B3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>3.42</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="D4" s="2">
         <v>1.6</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>6.5</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="D5" s="2">
         <v>1.93</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <f>C5/C4</f>
-        <v>1.9005847953216375</v>
-      </c>
-      <c r="D6">
+        <v>1.8823529411764708</v>
+      </c>
+      <c r="D6" s="2">
         <f>D5/D4</f>
         <v>1.2062499999999998</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>6000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>2200</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>6000</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
+        <v>25000</v>
+      </c>
+      <c r="D9" s="2">
         <v>4000</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>24000</v>
-      </c>
-      <c r="D9">
-        <v>4000</v>
-      </c>
-    </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <f>C9/C10</f>
-        <v>2400</v>
-      </c>
-      <c r="D11">
+        <v>2500</v>
+      </c>
+      <c r="D11" s="2">
         <f>D9/D10</f>
         <v>400</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <f>C9/C4</f>
-        <v>7017.5438596491231</v>
-      </c>
-      <c r="D12">
+        <v>7352.9411764705883</v>
+      </c>
+      <c r="D12" s="2">
         <f>D9/D4</f>
         <v>2500</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <f>1.1*C8</f>
         <v>6600.0000000000009</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <f>1.1*D8</f>
-        <v>4400</v>
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5">
+        <f>C6/C14</f>
+        <v>1.8823529411764709E-6</v>
+      </c>
+      <c r="D15" s="5">
+        <f>D6/D14</f>
+        <v>1.2062499999999999E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2">
+        <f>C12/10</f>
+        <v>735.29411764705878</v>
+      </c>
+      <c r="D16" s="2">
+        <f>D12/10</f>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>